<commit_message>
modified:   01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos.xlsx     srenamed:    03_Advanced_Internet_Programming/001.InteractiveCard/001.FilipeMatos/index.html -> 03_Advanced_Internet_Programming/Assignments/001.FilipeMatos/index.html  	renamed:    03_Advanced_Internet_Programming/001.InteractiveCard/001.FilipeMatos/style.css -> 03_Advanced_Internet_Programming/Assignments/001.FilipeMatos/style.css  	renamed:    03_Advanced_Internet_Programming/001.InteractiveCard/002.MiguelMagro/index.html -> 03_Advanced_Internet_Programming/Assignments/002.MiguelMagro/index.html  	renamed:    03_Advanced_Internet_Programming/001.InteractiveCard/002.MiguelMagro/style.css -> 03_Advanced_Internet_Programming/Assignments/002.MiguelMagro/style.css  	renamed:    03_Advanced_Internet_Programming/099.Lectures/Internet Programming.url -> 03_Advanced_Internet_Programming/Lectures/Internet Programming.url
</commit_message>
<xml_diff>
--- a/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos.xlsx
+++ b/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/201600728_estudantes_ips_pt/Documents/02. MEEC/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89B56B0D-932B-4A63-BBA9-A5E8206EE450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="8_{89B56B0D-932B-4A63-BBA9-A5E8206EE450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76895314-522F-4C6A-9623-E6419BAB7903}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="2" xr2:uid="{C8B6D815-6572-4EFD-9C5A-CC7C1F4CF928}"/>
+    <workbookView xWindow="43185" yWindow="-15" windowWidth="14430" windowHeight="15510" activeTab="1" xr2:uid="{C8B6D815-6572-4EFD-9C5A-CC7C1F4CF928}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Análise" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Vendas!$A$1:$N$37</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Vendas!$A$1:$O$37</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">Dicionário!$A$1:$B$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="120">
   <si>
     <t>VendaID</t>
   </si>
@@ -377,45 +377,79 @@
     <t>TicketClass</t>
   </si>
   <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>TotalPorVendedor</t>
-  </si>
-  <si>
-    <t>TotalPorRegiao</t>
-  </si>
-  <si>
-    <t>TicketMedioPorCat</t>
-  </si>
-  <si>
-    <t>Total Vendido por Vendedor na Região 'Lisboa'</t>
-  </si>
-  <si>
-    <t>Nº de Vendas na Catergoria 'Eletrónica'</t>
-  </si>
-  <si>
-    <t>Média Total 'Papelaria'</t>
+    <t>4.1 -TotalPorVendedor</t>
+  </si>
+  <si>
+    <t>4.2 - TotalPorRegiao</t>
+  </si>
+  <si>
+    <t>4.3 - TicketMedioPorCat</t>
+  </si>
+  <si>
+    <t>5.1 - Total Vendido por Vendedor na Região 'Lisboa'</t>
+  </si>
+  <si>
+    <t>5.2 - Nº de Vendas na Catergoria 'Eletrónica'</t>
+  </si>
+  <si>
+    <t>5.3 - Média Total 'Papelaria' 1º Trimestre</t>
+  </si>
+  <si>
+    <t>6.1 - 3 Maiores Vendas</t>
+  </si>
+  <si>
+    <t>6.2 - 3 Menores Vendas</t>
+  </si>
+  <si>
+    <t>7.1 - 3 Maiores Vendas</t>
+  </si>
+  <si>
+    <t>&gt;=150</t>
+  </si>
+  <si>
+    <t>1º Trimestre</t>
+  </si>
+  <si>
+    <t>Trimestre</t>
+  </si>
+  <si>
+    <t>Top Sales</t>
+  </si>
+  <si>
+    <t>Raking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raking </t>
+  </si>
+  <si>
+    <t>Designação</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>Prata</t>
+  </si>
+  <si>
+    <t>Ouro</t>
+  </si>
+  <si>
+    <t>Platina</t>
+  </si>
+  <si>
+    <t>EscalaCliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="175" formatCode="[$-816]mmmm"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-816]mmmm"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +467,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -472,12 +521,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,61 +553,62 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="177" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="[$-816]mmmm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -574,6 +624,35 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-816]mmmm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -594,6 +673,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="1" xr16:uid="{7436C19E-D99C-4C8C-A834-DE2D1035FB3C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="3">
@@ -607,13 +690,14 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{87DBE903-06DA-4FA9-9CF9-DEB543D27D80}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="26" unboundColumnsRight="9">
-    <queryTableFields count="23">
+  <queryTableRefresh nextId="27" unboundColumnsRight="4">
+    <queryTableFields count="19">
       <queryTableField id="1" name="VendaID" tableColumnId="1"/>
       <queryTableField id="2" name="Data" tableColumnId="2"/>
       <queryTableField id="13" dataBound="0" tableColumnId="14"/>
       <queryTableField id="12" dataBound="0" tableColumnId="13"/>
       <queryTableField id="15" dataBound="0" tableColumnId="16"/>
+      <queryTableField id="26" dataBound="0" tableColumnId="11"/>
       <queryTableField id="14" dataBound="0" tableColumnId="15"/>
       <queryTableField id="3" name="Cliente" tableColumnId="3"/>
       <queryTableField id="4" name="Região" tableColumnId="4"/>
@@ -627,11 +711,6 @@
       <queryTableField id="16" dataBound="0" tableColumnId="17"/>
       <queryTableField id="17" dataBound="0" tableColumnId="18"/>
       <queryTableField id="19" dataBound="0" tableColumnId="20"/>
-      <queryTableField id="20" dataBound="0" tableColumnId="21"/>
-      <queryTableField id="21" dataBound="0" tableColumnId="22"/>
-      <queryTableField id="22" dataBound="0" tableColumnId="23"/>
-      <queryTableField id="23" dataBound="0" tableColumnId="24"/>
-      <queryTableField id="24" dataBound="0" tableColumnId="25"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -641,54 +720,52 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{08C6DA56-6B3A-4899-9F3C-956E3B387568}" name="Dicionário" displayName="Dicionário" ref="A1:B12" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B12" xr:uid="{08C6DA56-6B3A-4899-9F3C-956E3B387568}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7F4A84EB-6B6D-4034-8C80-B10399C36DAB}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{25667AD9-7007-4548-9D81-9A0B436765B2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{7F4A84EB-6B6D-4034-8C80-B10399C36DAB}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{25667AD9-7007-4548-9D81-9A0B436765B2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C745892-CB11-480A-9A13-DF0FDB624DD6}" name="Vendas" displayName="Vendas" ref="A1:W37" tableType="queryTable" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:W37" xr:uid="{2C745892-CB11-480A-9A13-DF0FDB624DD6}"/>
-  <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{E2520904-6B5D-45F0-96C8-ACA51C110C87}" uniqueName="1" name="VendaID" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{92687A56-9717-4829-9D71-F850BE73C62D}" uniqueName="2" name="Data" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{2C81FA8E-EA36-4972-A8E1-5E7A918915C2}" uniqueName="14" name="Ano" queryTableFieldId="13" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C745892-CB11-480A-9A13-DF0FDB624DD6}" name="Vendas" displayName="Vendas" ref="A1:S37" tableType="queryTable" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:S37" xr:uid="{2C745892-CB11-480A-9A13-DF0FDB624DD6}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{E2520904-6B5D-45F0-96C8-ACA51C110C87}" uniqueName="1" name="VendaID" queryTableFieldId="1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{92687A56-9717-4829-9D71-F850BE73C62D}" uniqueName="2" name="Data" queryTableFieldId="2" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{2C81FA8E-EA36-4972-A8E1-5E7A918915C2}" uniqueName="14" name="Ano" queryTableFieldId="13" dataDxfId="12">
       <calculatedColumnFormula>TEXT(Vendas[[#This Row],[Data]],"aaaa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{44154506-83D6-4B91-9E63-6A835281EFFF}" uniqueName="13" name="Mês" queryTableFieldId="12" dataDxfId="7">
+    <tableColumn id="13" xr3:uid="{44154506-83D6-4B91-9E63-6A835281EFFF}" uniqueName="13" name="Mês" queryTableFieldId="12" dataDxfId="11">
       <calculatedColumnFormula>TEXT(Vendas[[#This Row],[Data]],"mm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{911A3605-294B-4411-A1C5-DDD3C21A95B6}" uniqueName="16" name="MêsNome" queryTableFieldId="15" dataDxfId="6">
+    <tableColumn id="16" xr3:uid="{911A3605-294B-4411-A1C5-DDD3C21A95B6}" uniqueName="16" name="MêsNome" queryTableFieldId="15" dataDxfId="10">
       <calculatedColumnFormula>TEXT(Vendas[[#This Row],[Data]],"mmmm")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{000F3AC2-80F8-471F-A1E3-8F25F829227E}" uniqueName="15" name="FimDoMês" queryTableFieldId="14" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{275B9828-61EB-4339-9C0E-BC9222ED70DE}" uniqueName="11" name="Trimestre" queryTableFieldId="26" dataDxfId="9">
+      <calculatedColumnFormula>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{000F3AC2-80F8-471F-A1E3-8F25F829227E}" uniqueName="15" name="FimDoMês" queryTableFieldId="14" dataDxfId="8">
       <calculatedColumnFormula>EOMONTH(Vendas[[#This Row],[Data]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00499A88-0632-43EE-B3DF-E3CBCFEFE59D}" uniqueName="3" name="Cliente" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{33FA48A6-EF28-4ABE-9F8C-F27F7CA78FD4}" uniqueName="4" name="Região" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{8B42700B-5DFA-4DCA-A1E0-9109EDC898A3}" uniqueName="5" name="Vendedor" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{BB060FDC-051E-44AF-ABCD-CD2D88BC8D8E}" uniqueName="6" name="Categoria" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{F5E9F08B-7FA8-4022-B775-41C325762E79}" uniqueName="7" name="Produto" queryTableFieldId="7" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00499A88-0632-43EE-B3DF-E3CBCFEFE59D}" uniqueName="3" name="Cliente" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{33FA48A6-EF28-4ABE-9F8C-F27F7CA78FD4}" uniqueName="4" name="Região" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8B42700B-5DFA-4DCA-A1E0-9109EDC898A3}" uniqueName="5" name="Vendedor" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{BB060FDC-051E-44AF-ABCD-CD2D88BC8D8E}" uniqueName="6" name="Categoria" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F5E9F08B-7FA8-4022-B775-41C325762E79}" uniqueName="7" name="Produto" queryTableFieldId="7" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{96F3CEA2-3D5D-48FF-93C3-987B367444DB}" uniqueName="8" name="Quantidade" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{4E39EFC5-477D-4217-A065-FE51B5134B8B}" uniqueName="9" name="PreçoUnitário" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{4E39EFC5-477D-4217-A065-FE51B5134B8B}" uniqueName="9" name="PreçoUnitário" queryTableFieldId="9" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{5AA078A0-1EEF-4DF2-9057-1322519CEF97}" uniqueName="10" name="Desconto(%)" queryTableFieldId="10"/>
-    <tableColumn id="12" xr3:uid="{B6981029-A6F9-4F62-92DF-4083EA0F37DE}" uniqueName="12" name="Total" queryTableFieldId="11" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{B6981029-A6F9-4F62-92DF-4083EA0F37DE}" uniqueName="12" name="Total" queryTableFieldId="11" dataCellStyle="Currency">
       <calculatedColumnFormula>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{D54BD190-66AC-4E6F-B05F-813E2B22C0CF}" uniqueName="17" name="DiasDesdeVenda" queryTableFieldId="16" dataDxfId="2">
+    <tableColumn id="17" xr3:uid="{D54BD190-66AC-4E6F-B05F-813E2B22C0CF}" uniqueName="17" name="DiasDesdeVenda" queryTableFieldId="16" dataDxfId="1">
       <calculatedColumnFormula>TODAY()-Vendas[[#This Row],[Data]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{04C47B09-F8D6-4181-8184-D348AA30E894}" uniqueName="18" name="TicketClass" queryTableFieldId="17" dataDxfId="3">
+    <tableColumn id="18" xr3:uid="{04C47B09-F8D6-4181-8184-D348AA30E894}" uniqueName="18" name="TicketClass" queryTableFieldId="17" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{CAD321CD-DB7D-4979-9DEB-93B32335347C}" uniqueName="20" name="TotalPorRegiao" queryTableFieldId="19"/>
-    <tableColumn id="21" xr3:uid="{F7E42F09-9F26-4BC9-8E38-7AC02D1CEE70}" uniqueName="21" name="TicketMedioPorCat" queryTableFieldId="20"/>
-    <tableColumn id="22" xr3:uid="{5FD55864-5B9D-4968-89E4-67D144CFC8A8}" uniqueName="22" name="Column4" queryTableFieldId="21"/>
-    <tableColumn id="23" xr3:uid="{9482442B-849C-4C0C-95C6-CB65C47BFC04}" uniqueName="23" name="Column5" queryTableFieldId="22"/>
-    <tableColumn id="24" xr3:uid="{FBEAC534-5EAB-4B59-A751-8B3690CF8FEA}" uniqueName="24" name="Column6" queryTableFieldId="23"/>
-    <tableColumn id="25" xr3:uid="{4CA0C342-FD46-46EB-878B-42968DCC8513}" uniqueName="25" name="Column7" queryTableFieldId="24"/>
+    <tableColumn id="20" xr3:uid="{CAD321CD-DB7D-4979-9DEB-93B32335347C}" uniqueName="20" name="EscalaCliente" queryTableFieldId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1015,13 +1092,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1029,91 +1106,91 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1127,2268 +1204,2400 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7013D5EB-BEF7-4A56-89FB-305F31E16D24}">
-  <dimension ref="A1:W47"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:H46"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection sqref="A1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.08203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.4140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="19.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.9140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="24" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" style="26" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="1" t="s">
+      <c r="S1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>45494</v>
       </c>
-      <c r="C2" s="7" t="str">
+      <c r="C2" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>07</v>
       </c>
-      <c r="E2" s="12" t="str">
+      <c r="E2" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>julho</v>
       </c>
       <c r="F2" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45504</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" t="s">
         <v>15</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>13</v>
       </c>
-      <c r="M2" s="15">
+      <c r="N2" s="13">
         <v>4.2300000000000004</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.15</v>
       </c>
-      <c r="O2" s="15">
+      <c r="P2" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>46.741500000000009</v>
       </c>
-      <c r="P2" s="7">
+      <c r="Q2" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>437</v>
-      </c>
-      <c r="Q2" t="str" cm="1">
-        <f t="array" ref="Q2">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>439</v>
+      </c>
+      <c r="R2" s="26" t="str" cm="1">
+        <f t="array" ref="R2">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>45495</v>
       </c>
-      <c r="C3" s="7" t="str">
+      <c r="C3" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D3" s="7" t="str">
+      <c r="D3" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>07</v>
       </c>
-      <c r="E3" s="12" t="str">
+      <c r="E3" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>julho</v>
       </c>
       <c r="F3" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45504</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="M3" s="15">
+      <c r="N3" s="13">
         <v>8.24</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="O3" s="15">
+      <c r="P3" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>32.96</v>
       </c>
-      <c r="P3" s="7">
+      <c r="Q3" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>436</v>
-      </c>
-      <c r="Q3" t="str" cm="1">
-        <f t="array" ref="Q3">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>438</v>
+      </c>
+      <c r="R3" s="26" t="str" cm="1">
+        <f t="array" ref="R3">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>45522</v>
       </c>
-      <c r="C4" s="7" t="str">
+      <c r="C4" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="D4" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>08</v>
       </c>
-      <c r="E4" s="12" t="str">
+      <c r="E4" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>agosto</v>
       </c>
       <c r="F4" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45535</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" t="s">
         <v>22</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="M4" s="15">
+      <c r="N4" s="13">
         <v>4.22</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.05</v>
       </c>
-      <c r="O4" s="15">
+      <c r="P4" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>12.026999999999999</v>
       </c>
-      <c r="P4" s="7">
+      <c r="Q4" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>409</v>
-      </c>
-      <c r="Q4" t="str" cm="1">
-        <f t="array" ref="Q4">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>411</v>
+      </c>
+      <c r="R4" s="26" t="str" cm="1">
+        <f t="array" ref="R4">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>45532</v>
       </c>
-      <c r="C5" s="7" t="str">
+      <c r="C5" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D5" s="7" t="str">
+      <c r="D5" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>08</v>
       </c>
-      <c r="E5" s="12" t="str">
+      <c r="E5" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>agosto</v>
       </c>
       <c r="F5" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G5" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45535</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="M5" s="15">
+      <c r="N5" s="13">
         <v>7.38</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.15</v>
       </c>
-      <c r="O5" s="15">
+      <c r="P5" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>6.2729999999999997</v>
       </c>
-      <c r="P5" s="7">
+      <c r="Q5" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>399</v>
-      </c>
-      <c r="Q5" t="str" cm="1">
-        <f t="array" ref="Q5">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>401</v>
+      </c>
+      <c r="R5" s="26" t="str" cm="1">
+        <f t="array" ref="R5">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>45545</v>
       </c>
-      <c r="C6" s="7" t="str">
+      <c r="C6" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>09</v>
       </c>
-      <c r="E6" s="12" t="str">
+      <c r="E6" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>setembro</v>
       </c>
       <c r="F6" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45565</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" t="s">
         <v>28</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>4</v>
       </c>
-      <c r="M6" s="15">
+      <c r="N6" s="13">
         <v>11.35</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.05</v>
       </c>
-      <c r="O6" s="15">
+      <c r="P6" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>43.129999999999995</v>
       </c>
-      <c r="P6" s="7">
+      <c r="Q6" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>386</v>
-      </c>
-      <c r="Q6" t="str" cm="1">
-        <f t="array" ref="Q6">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>388</v>
+      </c>
+      <c r="R6" s="26" t="str" cm="1">
+        <f t="array" ref="R6">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>45561</v>
       </c>
-      <c r="C7" s="7" t="str">
+      <c r="C7" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D7" s="7" t="str">
+      <c r="D7" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>09</v>
       </c>
-      <c r="E7" s="12" t="str">
+      <c r="E7" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>setembro</v>
       </c>
       <c r="F7" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45565</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" t="s">
         <v>20</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>10</v>
       </c>
-      <c r="M7" s="15">
+      <c r="N7" s="13">
         <v>6.85</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.1</v>
       </c>
-      <c r="O7" s="15">
+      <c r="P7" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>61.65</v>
       </c>
-      <c r="P7" s="7">
+      <c r="Q7" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>370</v>
-      </c>
-      <c r="Q7" t="str" cm="1">
-        <f t="array" ref="Q7">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>372</v>
+      </c>
+      <c r="R7" s="26" t="str" cm="1">
+        <f t="array" ref="R7">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>45573</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C8" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="D8" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>10</v>
       </c>
-      <c r="E8" s="12" t="str">
+      <c r="E8" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>outubro</v>
       </c>
       <c r="F8" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45596</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" t="s">
         <v>33</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>2</v>
       </c>
-      <c r="M8" s="15">
+      <c r="N8" s="13">
         <v>33.71</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0.15</v>
       </c>
-      <c r="O8" s="15">
+      <c r="P8" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>57.307000000000002</v>
       </c>
-      <c r="P8" s="7">
+      <c r="Q8" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>358</v>
-      </c>
-      <c r="Q8" t="str" cm="1">
-        <f t="array" ref="Q8">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>360</v>
+      </c>
+      <c r="R8" s="26" t="str" cm="1">
+        <f t="array" ref="R8">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>45576</v>
       </c>
-      <c r="C9" s="7" t="str">
+      <c r="C9" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D9" s="7" t="str">
+      <c r="D9" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>10</v>
       </c>
-      <c r="E9" s="12" t="str">
+      <c r="E9" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>outubro</v>
       </c>
       <c r="F9" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45596</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" t="s">
         <v>37</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>16</v>
       </c>
-      <c r="M9" s="15">
+      <c r="N9" s="13">
         <v>3.22</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.15</v>
       </c>
-      <c r="O9" s="15">
+      <c r="P9" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>43.792000000000002</v>
       </c>
-      <c r="P9" s="7">
+      <c r="Q9" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>355</v>
-      </c>
-      <c r="Q9" t="str" cm="1">
-        <f t="array" ref="Q9">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>357</v>
+      </c>
+      <c r="R9" s="26" t="str" cm="1">
+        <f t="array" ref="R9">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>45576</v>
       </c>
-      <c r="C10" s="7" t="str">
+      <c r="C10" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D10" s="7" t="str">
+      <c r="D10" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>10</v>
       </c>
-      <c r="E10" s="12" t="str">
+      <c r="E10" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>outubro</v>
       </c>
       <c r="F10" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45596</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" t="s">
         <v>39</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>8</v>
       </c>
-      <c r="M10" s="15">
+      <c r="N10" s="13">
         <v>36.57</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.15</v>
       </c>
-      <c r="O10" s="15">
+      <c r="P10" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>248.67599999999999</v>
       </c>
-      <c r="P10" s="7">
+      <c r="Q10" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>355</v>
-      </c>
-      <c r="Q10" t="str" cm="1">
-        <f t="array" ref="Q10">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>357</v>
+      </c>
+      <c r="R10" s="26" t="str" cm="1">
+        <f t="array" ref="R10">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>45580</v>
       </c>
-      <c r="C11" s="7" t="str">
+      <c r="C11" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D11" s="7" t="str">
+      <c r="D11" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>10</v>
       </c>
-      <c r="E11" s="12" t="str">
+      <c r="E11" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>outubro</v>
       </c>
       <c r="F11" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45596</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" t="s">
         <v>28</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>22</v>
       </c>
-      <c r="M11" s="15">
+      <c r="N11" s="13">
         <v>4.57</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.05</v>
       </c>
-      <c r="O11" s="15">
+      <c r="P11" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>95.513000000000005</v>
       </c>
-      <c r="P11" s="7">
+      <c r="Q11" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>351</v>
-      </c>
-      <c r="Q11" t="str" cm="1">
-        <f t="array" ref="Q11">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>353</v>
+      </c>
+      <c r="R11" s="26" t="str" cm="1">
+        <f t="array" ref="R11">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>45595</v>
       </c>
-      <c r="C12" s="7" t="str">
+      <c r="C12" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D12" s="7" t="str">
+      <c r="D12" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>10</v>
       </c>
-      <c r="E12" s="12" t="str">
+      <c r="E12" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>outubro</v>
       </c>
       <c r="F12" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45596</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" t="s">
         <v>43</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>10</v>
       </c>
-      <c r="M12" s="15">
+      <c r="N12" s="13">
         <v>14.45</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0</v>
       </c>
-      <c r="O12" s="15">
+      <c r="P12" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>144.5</v>
       </c>
-      <c r="P12" s="7">
+      <c r="Q12" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>336</v>
-      </c>
-      <c r="Q12" t="str" cm="1">
-        <f t="array" ref="Q12">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>338</v>
+      </c>
+      <c r="R12" s="26" t="str" cm="1">
+        <f t="array" ref="R12">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>45604</v>
       </c>
-      <c r="C13" s="7" t="str">
+      <c r="C13" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D13" s="7" t="str">
+      <c r="D13" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>11</v>
       </c>
-      <c r="E13" s="12" t="str">
+      <c r="E13" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>novembro</v>
       </c>
       <c r="F13" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G13" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45626</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" t="s">
         <v>39</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>8</v>
       </c>
-      <c r="M13" s="15">
+      <c r="N13" s="13">
         <v>19.28</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.05</v>
       </c>
-      <c r="O13" s="15">
+      <c r="P13" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>146.52799999999999</v>
       </c>
-      <c r="P13" s="7">
+      <c r="Q13" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>327</v>
-      </c>
-      <c r="Q13" t="str" cm="1">
-        <f t="array" ref="Q13">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>329</v>
+      </c>
+      <c r="R13" s="26" t="str" cm="1">
+        <f t="array" ref="R13">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>45623</v>
       </c>
-      <c r="C14" s="7" t="str">
+      <c r="C14" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D14" s="7" t="str">
+      <c r="D14" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>11</v>
       </c>
-      <c r="E14" s="12" t="str">
+      <c r="E14" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>novembro</v>
       </c>
       <c r="F14" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G14" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45626</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" t="s">
         <v>36</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" t="s">
         <v>37</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>22</v>
       </c>
-      <c r="M14" s="15">
+      <c r="N14" s="13">
         <v>7.73</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>0.1</v>
       </c>
-      <c r="O14" s="15">
+      <c r="P14" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>153.054</v>
       </c>
-      <c r="P14" s="7">
+      <c r="Q14" s="6">
+        <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
+        <v>310</v>
+      </c>
+      <c r="R14" s="26" t="str" cm="1">
+        <f t="array" ref="R14">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>Médio</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45625</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
+        <v>2024</v>
+      </c>
+      <c r="D15" s="19" t="str">
+        <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
+        <v>11</v>
+      </c>
+      <c r="E15" s="11" t="str">
+        <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
+        <v>novembro</v>
+      </c>
+      <c r="F15" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
+        <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
+        <v>45626</v>
+      </c>
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" s="13">
+        <v>8.02</v>
+      </c>
+      <c r="O15">
+        <v>0.05</v>
+      </c>
+      <c r="P15" s="24">
+        <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
+        <v>7.6189999999999989</v>
+      </c>
+      <c r="Q15" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
         <v>308</v>
       </c>
-      <c r="Q14" t="str" cm="1">
-        <f t="array" ref="Q14">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
-        <v>Médio</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="2">
-        <v>45625</v>
-      </c>
-      <c r="C15" s="7" t="str">
+      <c r="R15" s="26" t="str" cm="1">
+        <f t="array" ref="R15">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>Baixo</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45634</v>
+      </c>
+      <c r="C16" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2024</v>
       </c>
-      <c r="D15" s="7" t="str">
-        <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
-        <v>11</v>
-      </c>
-      <c r="E15" s="12" t="str">
-        <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
-        <v>novembro</v>
-      </c>
-      <c r="F15" s="6">
-        <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
-        <v>45626</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15" s="15">
-        <v>8.02</v>
-      </c>
-      <c r="N15">
-        <v>0.05</v>
-      </c>
-      <c r="O15" s="15">
-        <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
-        <v>7.6189999999999989</v>
-      </c>
-      <c r="P15" s="7">
-        <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>306</v>
-      </c>
-      <c r="Q15" t="str" cm="1">
-        <f t="array" ref="Q15">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
-        <v>Baixo</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="2">
-        <v>45634</v>
-      </c>
-      <c r="C16" s="7" t="str">
-        <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
-        <v>2024</v>
-      </c>
-      <c r="D16" s="7" t="str">
+      <c r="D16" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>12</v>
       </c>
-      <c r="E16" s="12" t="str">
+      <c r="E16" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>dezembro</v>
       </c>
       <c r="F16" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G16" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45657</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" t="s">
         <v>15</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>17</v>
       </c>
-      <c r="M16" s="15">
+      <c r="N16" s="13">
         <v>8.1300000000000008</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>0.1</v>
       </c>
-      <c r="O16" s="15">
+      <c r="P16" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>124.38900000000001</v>
       </c>
-      <c r="P16" s="7">
+      <c r="Q16" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>297</v>
-      </c>
-      <c r="Q16" t="str" cm="1">
-        <f t="array" ref="Q16">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>299</v>
+      </c>
+      <c r="R16" s="26" t="str" cm="1">
+        <f t="array" ref="R16">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>45662</v>
       </c>
-      <c r="C17" s="7" t="str">
+      <c r="C17" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D17" s="7" t="str">
+      <c r="D17" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>01</v>
       </c>
-      <c r="E17" s="12" t="str">
+      <c r="E17" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>janeiro</v>
       </c>
       <c r="F17" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45688</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" t="s">
         <v>28</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>21</v>
       </c>
-      <c r="M17" s="15">
+      <c r="N17" s="13">
         <v>1.69</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>0.15</v>
       </c>
-      <c r="O17" s="15">
+      <c r="P17" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>30.166499999999999</v>
       </c>
-      <c r="P17" s="7">
+      <c r="Q17" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>269</v>
-      </c>
-      <c r="Q17" t="str" cm="1">
-        <f t="array" ref="Q17">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>271</v>
+      </c>
+      <c r="R17" s="26" t="str" cm="1">
+        <f t="array" ref="R17">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>45665</v>
       </c>
-      <c r="C18" s="7" t="str">
+      <c r="C18" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D18" s="7" t="str">
+      <c r="D18" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>01</v>
       </c>
-      <c r="E18" s="12" t="str">
+      <c r="E18" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>janeiro</v>
       </c>
       <c r="F18" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45688</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" t="s">
         <v>15</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>18</v>
       </c>
-      <c r="M18" s="15">
+      <c r="N18" s="13">
         <v>8.5</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>0</v>
       </c>
-      <c r="O18" s="15">
+      <c r="P18" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>153</v>
       </c>
-      <c r="P18" s="7">
+      <c r="Q18" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>266</v>
-      </c>
-      <c r="Q18" t="str" cm="1">
-        <f t="array" ref="Q18">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>268</v>
+      </c>
+      <c r="R18" s="26" t="str" cm="1">
+        <f t="array" ref="R18">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>45688</v>
       </c>
-      <c r="C19" s="7" t="str">
+      <c r="C19" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D19" s="7" t="str">
+      <c r="D19" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>01</v>
       </c>
-      <c r="E19" s="12" t="str">
+      <c r="E19" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>janeiro</v>
       </c>
       <c r="F19" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45688</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" t="s">
         <v>56</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>23</v>
       </c>
-      <c r="M19" s="15">
+      <c r="N19" s="13">
         <v>20.239999999999998</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>0.15</v>
       </c>
-      <c r="O19" s="15">
+      <c r="P19" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>395.69199999999995</v>
       </c>
-      <c r="P19" s="7">
+      <c r="Q19" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>243</v>
-      </c>
-      <c r="Q19" t="str" cm="1">
-        <f t="array" ref="Q19">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>245</v>
+      </c>
+      <c r="R19" s="26" t="str" cm="1">
+        <f t="array" ref="R19">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Alto</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>45709</v>
       </c>
-      <c r="C20" s="7" t="str">
+      <c r="C20" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D20" s="7" t="str">
+      <c r="D20" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>02</v>
       </c>
-      <c r="E20" s="12" t="str">
+      <c r="E20" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>fevereiro</v>
       </c>
       <c r="F20" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45716</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" t="s">
         <v>22</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>2</v>
       </c>
-      <c r="M20" s="15">
+      <c r="N20" s="13">
         <v>6.46</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>0.15</v>
       </c>
-      <c r="O20" s="15">
+      <c r="P20" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>10.981999999999999</v>
       </c>
-      <c r="P20" s="7">
+      <c r="Q20" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>222</v>
-      </c>
-      <c r="Q20" t="str" cm="1">
-        <f t="array" ref="Q20">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>224</v>
+      </c>
+      <c r="R20" s="26" t="str" cm="1">
+        <f t="array" ref="R20">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>45726</v>
       </c>
-      <c r="C21" s="7" t="str">
+      <c r="C21" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="D21" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>03</v>
       </c>
-      <c r="E21" s="12" t="str">
+      <c r="E21" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>março</v>
       </c>
       <c r="F21" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45747</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" t="s">
         <v>43</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>16</v>
       </c>
-      <c r="M21" s="15">
+      <c r="N21" s="13">
         <v>12.69</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>0</v>
       </c>
-      <c r="O21" s="15">
+      <c r="P21" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>203.04</v>
       </c>
-      <c r="P21" s="7">
+      <c r="Q21" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>205</v>
-      </c>
-      <c r="Q21" t="str" cm="1">
-        <f t="array" ref="Q21">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>207</v>
+      </c>
+      <c r="R21" s="26" t="str" cm="1">
+        <f t="array" ref="R21">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>45731</v>
       </c>
-      <c r="C22" s="7" t="str">
+      <c r="C22" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D22" s="7" t="str">
+      <c r="D22" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>03</v>
       </c>
-      <c r="E22" s="12" t="str">
+      <c r="E22" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>março</v>
       </c>
       <c r="F22" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45747</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" t="s">
         <v>33</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>22</v>
       </c>
-      <c r="M22" s="15">
+      <c r="N22" s="13">
         <v>30.55</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>0.05</v>
       </c>
-      <c r="O22" s="15">
+      <c r="P22" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>638.495</v>
       </c>
-      <c r="P22" s="7">
+      <c r="Q22" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>200</v>
-      </c>
-      <c r="Q22" t="str" cm="1">
-        <f t="array" ref="Q22">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>202</v>
+      </c>
+      <c r="R22" s="26" t="str" cm="1">
+        <f t="array" ref="R22">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Alto</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>45744</v>
       </c>
-      <c r="C23" s="7" t="str">
+      <c r="C23" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D23" s="7" t="str">
+      <c r="D23" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>03</v>
       </c>
-      <c r="E23" s="12" t="str">
+      <c r="E23" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>março</v>
       </c>
       <c r="F23" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45747</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" t="s">
         <v>50</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>8</v>
       </c>
-      <c r="M23" s="15">
+      <c r="N23" s="13">
         <v>4.3899999999999997</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>0</v>
       </c>
-      <c r="O23" s="15">
+      <c r="P23" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>35.119999999999997</v>
       </c>
-      <c r="P23" s="7">
+      <c r="Q23" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>187</v>
-      </c>
-      <c r="Q23" t="str" cm="1">
-        <f t="array" ref="Q23">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>189</v>
+      </c>
+      <c r="R23" s="26" t="str" cm="1">
+        <f t="array" ref="R23">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>45750</v>
       </c>
-      <c r="C24" s="7" t="str">
+      <c r="C24" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D24" s="7" t="str">
+      <c r="D24" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>04</v>
       </c>
-      <c r="E24" s="12" t="str">
+      <c r="E24" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>abril</v>
       </c>
       <c r="F24" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G24" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45777</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" t="s">
         <v>33</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>3</v>
       </c>
-      <c r="M24" s="15">
+      <c r="N24" s="13">
         <v>14.98</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>0</v>
       </c>
-      <c r="O24" s="15">
+      <c r="P24" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>44.94</v>
       </c>
-      <c r="P24" s="7">
+      <c r="Q24" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>181</v>
-      </c>
-      <c r="Q24" t="str" cm="1">
-        <f t="array" ref="Q24">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>183</v>
+      </c>
+      <c r="R24" s="26" t="str" cm="1">
+        <f t="array" ref="R24">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>45767</v>
       </c>
-      <c r="C25" s="7" t="str">
+      <c r="C25" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D25" s="7" t="str">
+      <c r="D25" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>04</v>
       </c>
-      <c r="E25" s="12" t="str">
+      <c r="E25" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>abril</v>
       </c>
       <c r="F25" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G25" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45777</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" t="s">
         <v>47</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" t="s">
         <v>56</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>3</v>
       </c>
-      <c r="M25" s="15">
+      <c r="N25" s="13">
         <v>26.8</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.15</v>
       </c>
-      <c r="O25" s="15">
+      <c r="P25" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>68.34</v>
       </c>
-      <c r="P25" s="7">
+      <c r="Q25" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>164</v>
-      </c>
-      <c r="Q25" t="str" cm="1">
-        <f t="array" ref="Q25">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>166</v>
+      </c>
+      <c r="R25" s="26" t="str" cm="1">
+        <f t="array" ref="R25">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>45782</v>
       </c>
-      <c r="C26" s="7" t="str">
+      <c r="C26" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D26" s="7" t="str">
+      <c r="D26" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>05</v>
       </c>
-      <c r="E26" s="12" t="str">
+      <c r="E26" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>maio</v>
       </c>
       <c r="F26" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G26" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45808</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" t="s">
         <v>39</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>7</v>
       </c>
-      <c r="M26" s="15">
+      <c r="N26" s="13">
         <v>17.39</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>0.15</v>
       </c>
-      <c r="O26" s="15">
+      <c r="P26" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>103.4705</v>
       </c>
-      <c r="P26" s="7">
+      <c r="Q26" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>149</v>
-      </c>
-      <c r="Q26" t="str" cm="1">
-        <f t="array" ref="Q26">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>151</v>
+      </c>
+      <c r="R26" s="26" t="str" cm="1">
+        <f t="array" ref="R26">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>45787</v>
       </c>
-      <c r="C27" s="7" t="str">
+      <c r="C27" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D27" s="7" t="str">
+      <c r="D27" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>05</v>
       </c>
-      <c r="E27" s="12" t="str">
+      <c r="E27" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>maio</v>
       </c>
       <c r="F27" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G27" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45808</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" t="s">
         <v>20</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>3</v>
       </c>
-      <c r="M27" s="15">
+      <c r="N27" s="13">
         <v>5.22</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>0</v>
       </c>
-      <c r="O27" s="15">
+      <c r="P27" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>15.66</v>
       </c>
-      <c r="P27" s="7">
+      <c r="Q27" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>144</v>
-      </c>
-      <c r="Q27" t="str" cm="1">
-        <f t="array" ref="Q27">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>146</v>
+      </c>
+      <c r="R27" s="26" t="str" cm="1">
+        <f t="array" ref="R27">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>45804</v>
       </c>
-      <c r="C28" s="7" t="str">
+      <c r="C28" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D28" s="7" t="str">
+      <c r="D28" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>05</v>
       </c>
-      <c r="E28" s="12" t="str">
+      <c r="E28" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>maio</v>
       </c>
       <c r="F28" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G28" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45808</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" t="s">
         <v>13</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" t="s">
         <v>20</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>5</v>
       </c>
-      <c r="M28" s="15">
+      <c r="N28" s="13">
         <v>7.26</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>0.1</v>
       </c>
-      <c r="O28" s="15">
+      <c r="P28" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>32.67</v>
       </c>
-      <c r="P28" s="7">
+      <c r="Q28" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>127</v>
-      </c>
-      <c r="Q28" t="str" cm="1">
-        <f t="array" ref="Q28">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>129</v>
+      </c>
+      <c r="R28" s="26" t="str" cm="1">
+        <f t="array" ref="R28">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>45817</v>
       </c>
-      <c r="C29" s="7" t="str">
+      <c r="C29" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D29" s="7" t="str">
+      <c r="D29" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>06</v>
       </c>
-      <c r="E29" s="12" t="str">
+      <c r="E29" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>junho</v>
       </c>
       <c r="F29" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G29" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45838</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" t="s">
         <v>47</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" t="s">
         <v>36</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" t="s">
         <v>37</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>6</v>
       </c>
-      <c r="M29" s="15">
+      <c r="N29" s="13">
         <v>10.73</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>0.05</v>
       </c>
-      <c r="O29" s="15">
+      <c r="P29" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>61.160999999999994</v>
       </c>
-      <c r="P29" s="7">
+      <c r="Q29" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>114</v>
-      </c>
-      <c r="Q29" t="str" cm="1">
-        <f t="array" ref="Q29">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>116</v>
+      </c>
+      <c r="R29" s="26" t="str" cm="1">
+        <f t="array" ref="R29">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>45818</v>
       </c>
-      <c r="C30" s="7" t="str">
+      <c r="C30" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D30" s="7" t="str">
+      <c r="D30" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>06</v>
       </c>
-      <c r="E30" s="12" t="str">
+      <c r="E30" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>junho</v>
       </c>
       <c r="F30" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G30" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45838</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" t="s">
         <v>47</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" t="s">
         <v>56</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>4</v>
       </c>
-      <c r="M30" s="15">
+      <c r="N30" s="13">
         <v>34.729999999999997</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>0.1</v>
       </c>
-      <c r="O30" s="15">
+      <c r="P30" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>125.02799999999999</v>
       </c>
-      <c r="P30" s="7">
+      <c r="Q30" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>113</v>
-      </c>
-      <c r="Q30" t="str" cm="1">
-        <f t="array" ref="Q30">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>115</v>
+      </c>
+      <c r="R30" s="26" t="str" cm="1">
+        <f t="array" ref="R30">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>45822</v>
       </c>
-      <c r="C31" s="7" t="str">
+      <c r="C31" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D31" s="7" t="str">
+      <c r="D31" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>06</v>
       </c>
-      <c r="E31" s="12" t="str">
+      <c r="E31" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>junho</v>
       </c>
       <c r="F31" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G31" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45838</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" t="s">
         <v>28</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>18</v>
       </c>
-      <c r="M31" s="15">
+      <c r="N31" s="13">
         <v>11.38</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>0.05</v>
       </c>
-      <c r="O31" s="15">
+      <c r="P31" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>194.59799999999998</v>
       </c>
-      <c r="P31" s="7">
+      <c r="Q31" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>109</v>
-      </c>
-      <c r="Q31" t="str" cm="1">
-        <f t="array" ref="Q31">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>111</v>
+      </c>
+      <c r="R31" s="26" t="str" cm="1">
+        <f t="array" ref="R31">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>45833</v>
       </c>
-      <c r="C32" s="7" t="str">
+      <c r="C32" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D32" s="7" t="str">
+      <c r="D32" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>06</v>
       </c>
-      <c r="E32" s="12" t="str">
+      <c r="E32" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>junho</v>
       </c>
       <c r="F32" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G32" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45838</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" t="s">
         <v>71</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" t="s">
         <v>25</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" t="s">
         <v>14</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" t="s">
         <v>28</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>20</v>
       </c>
-      <c r="M32" s="15">
+      <c r="N32" s="13">
         <v>9.8800000000000008</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>0.15</v>
       </c>
-      <c r="O32" s="15">
+      <c r="P32" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>167.96</v>
       </c>
-      <c r="P32" s="7">
+      <c r="Q32" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>98</v>
-      </c>
-      <c r="Q32" t="str" cm="1">
-        <f t="array" ref="Q32">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>100</v>
+      </c>
+      <c r="R32" s="26" t="str" cm="1">
+        <f t="array" ref="R32">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>45846</v>
       </c>
-      <c r="C33" s="7" t="str">
+      <c r="C33" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D33" s="7" t="str">
+      <c r="D33" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>07</v>
       </c>
-      <c r="E33" s="12" t="str">
+      <c r="E33" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>julho</v>
       </c>
       <c r="F33" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G33" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45869</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" t="s">
         <v>46</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" t="s">
         <v>25</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" t="s">
         <v>56</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>5</v>
       </c>
-      <c r="M33" s="15">
+      <c r="N33" s="13">
         <v>28.84</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>0.15</v>
       </c>
-      <c r="O33" s="15">
+      <c r="P33" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>122.57</v>
       </c>
-      <c r="P33" s="7">
+      <c r="Q33" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>85</v>
-      </c>
-      <c r="Q33" t="str" cm="1">
-        <f t="array" ref="Q33">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>87</v>
+      </c>
+      <c r="R33" s="26" t="str" cm="1">
+        <f t="array" ref="R33">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Médio</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>45859</v>
       </c>
-      <c r="C34" s="7" t="str">
+      <c r="C34" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D34" s="7" t="str">
+      <c r="D34" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>07</v>
       </c>
-      <c r="E34" s="12" t="str">
+      <c r="E34" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>julho</v>
       </c>
       <c r="F34" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G34" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45869</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" t="s">
         <v>47</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" t="s">
         <v>20</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>7</v>
       </c>
-      <c r="M34" s="15">
+      <c r="N34" s="13">
         <v>9.94</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>0.15</v>
       </c>
-      <c r="O34" s="15">
+      <c r="P34" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>59.142999999999994</v>
       </c>
-      <c r="P34" s="7">
+      <c r="Q34" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>72</v>
-      </c>
-      <c r="Q34" t="str" cm="1">
-        <f t="array" ref="Q34">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>74</v>
+      </c>
+      <c r="R34" s="26" t="str" cm="1">
+        <f t="array" ref="R34">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>45887</v>
       </c>
-      <c r="C35" s="7" t="str">
+      <c r="C35" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D35" s="7" t="str">
+      <c r="D35" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>08</v>
       </c>
-      <c r="E35" s="12" t="str">
+      <c r="E35" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>agosto</v>
       </c>
       <c r="F35" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G35" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45900</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" t="s">
         <v>47</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" t="s">
         <v>75</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>5</v>
       </c>
-      <c r="M35" s="15">
+      <c r="N35" s="13">
         <v>13.79</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>0.15</v>
       </c>
-      <c r="O35" s="15">
+      <c r="P35" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>58.607499999999987</v>
       </c>
-      <c r="P35" s="7">
+      <c r="Q35" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>44</v>
-      </c>
-      <c r="Q35" t="str" cm="1">
-        <f t="array" ref="Q35">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>46</v>
+      </c>
+      <c r="R35" s="26" t="str" cm="1">
+        <f t="array" ref="R35">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>45909</v>
       </c>
-      <c r="C36" s="7" t="str">
+      <c r="C36" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D36" s="7" t="str">
+      <c r="D36" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>09</v>
       </c>
-      <c r="E36" s="12" t="str">
+      <c r="E36" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>setembro</v>
       </c>
       <c r="F36" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G36" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45930</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" t="s">
         <v>19</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" t="s">
         <v>36</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" t="s">
         <v>50</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>5</v>
       </c>
-      <c r="M36" s="15">
+      <c r="N36" s="13">
         <v>11.68</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>0.1</v>
       </c>
-      <c r="O36" s="15">
+      <c r="P36" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>52.56</v>
       </c>
-      <c r="P36" s="7">
+      <c r="Q36" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>22</v>
-      </c>
-      <c r="Q36" t="str" cm="1">
-        <f t="array" ref="Q36">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>24</v>
+      </c>
+      <c r="R36" s="26" t="str" cm="1">
+        <f t="array" ref="R36">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>45917</v>
       </c>
-      <c r="C37" s="7" t="str">
+      <c r="C37" s="6" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"aaaa")</f>
         <v>2025</v>
       </c>
-      <c r="D37" s="7" t="str">
+      <c r="D37" s="19" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mm")</f>
         <v>09</v>
       </c>
-      <c r="E37" s="12" t="str">
+      <c r="E37" s="11" t="str">
         <f>TEXT(Vendas[[#This Row],[Data]],"mmmm")</f>
         <v>setembro</v>
       </c>
       <c r="F37" s="6">
+        <f>ROUNDUP(MONTH(Vendas[[#This Row],[Data]])/3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G37" s="5">
         <f>EOMONTH(Vendas[[#This Row],[Data]],0)</f>
         <v>45930</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" t="s">
         <v>19</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" t="s">
         <v>36</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" t="s">
         <v>50</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>20</v>
       </c>
-      <c r="M37" s="15">
+      <c r="N37" s="13">
         <v>5.21</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>0.15</v>
       </c>
-      <c r="O37" s="15">
+      <c r="P37" s="24">
         <f>Vendas[[#This Row],[Quantidade]]*Vendas[[#This Row],[PreçoUnitário]]*(1-Vendas[[#This Row],[Desconto(%)]])</f>
         <v>88.57</v>
       </c>
-      <c r="P37" s="7">
+      <c r="Q37" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>14</v>
-      </c>
-      <c r="Q37" t="str" cm="1">
-        <f t="array" ref="Q37">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
+        <v>16</v>
+      </c>
+      <c r="R37" s="26" t="str" cm="1">
+        <f t="array" ref="R37">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
         <v>Baixo</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
-      <c r="D47" s="14"/>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D47" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3402,188 +3611,572 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E298A1-41BF-485F-AE78-098E1D130449}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.4140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="13" t="s">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="L1" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <f>SUMIF(Vendas[Vendedor],A2,Vendas[Quantidade])</f>
         <v>131</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="7">
-        <f>COUNTIF(Vendas[Região],D2)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="15">
-        <f>AVERAGEIF(Vendas[Categoria],G2,Vendas[Total])</f>
-        <v>195.10464999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="C2" s="6"/>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="13">
+        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!D2,Vendas[Região],$A$12)</f>
+        <v>326.90999999999997</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <f>SUMIF(Vendas[Vendedor],A3,Vendas[Quantidade])</f>
         <v>102</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="7">
-        <f>COUNTIF(Vendas[Região],D3)</f>
-        <v>3</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="15">
-        <f>AVERAGEIF(Vendas[Categoria],G3,Vendas[Total])</f>
-        <v>84.802349999999976</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="C3" s="6"/>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="13">
+        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!D3,Vendas[Região],$A$12)</f>
+        <v>249.99849999999998</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="21">
+        <v>1</v>
+      </c>
+      <c r="H3" s="24">
+        <f>_xlfn.NUMBERVALUE(LARGE(Vendas[Total],G3))</f>
+        <v>638.495</v>
+      </c>
+      <c r="I3" s="22" t="e">
+        <f>LOOKUP(H3,Vendas[])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J3" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H$3,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <f>SUMIF(Vendas[Vendedor],A4,Vendas[Quantidade])</f>
         <v>50</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="7">
-        <f>COUNTIF(Vendas[Região],D4)</f>
-        <v>7</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="15">
-        <f>AVERAGEIF(Vendas[Categoria],G4,Vendas[Total])</f>
-        <v>67.928937499999989</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="C4" s="6"/>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="13">
+        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!D4,Vendas[Região],$A$12)</f>
+        <v>126.94749999999999</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="21">
+        <v>2</v>
+      </c>
+      <c r="H4" s="24">
+        <f>_xlfn.NUMBERVALUE(LARGE(Vendas[Total],G4))</f>
+        <v>395.69200000000001</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H4,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+      <c r="M4" s="2">
+        <v>100</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <f>SUMIF(Vendas[Vendedor],A5,Vendas[Quantidade])</f>
         <v>79</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="13">
+        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!D5,Vendas[Região],$A$12)</f>
+        <v>100.09699999999999</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="24">
+        <f>_xlfn.NUMBERVALUE(LARGE(Vendas[Total],G5))</f>
+        <v>248.67599999999999</v>
+      </c>
+      <c r="I5" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H5,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+      <c r="J5" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H5,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+      <c r="M5" s="2">
+        <v>200</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="6"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="13"/>
+      <c r="M6" s="2">
+        <v>350</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="3">
+        <f>COUNTIF(Vendas[Região],A9)</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="6">
+        <f>COUNTIFS(Vendas[Categoria],A17,Vendas[Total],D9)</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3">
+        <f>COUNTIF(Vendas[Região],A10)</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24">
+        <f>_xlfn.NUMBERVALUE(SMALL(Vendas[Total],G10))</f>
+        <v>6.2729999999999997</v>
+      </c>
+      <c r="I10" s="22" t="e">
+        <f>LOOKUP(H10,Vendas[])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J10" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H10,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3">
+        <f>COUNTIF(Vendas[Região],A11)</f>
+        <v>7</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="21">
+        <v>2</v>
+      </c>
+      <c r="H11" s="24">
+        <f>_xlfn.NUMBERVALUE(SMALL(Vendas[Total],G11))</f>
+        <v>7.6189999999999998</v>
+      </c>
+      <c r="I11" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H11,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+      <c r="J11" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H11,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="7">
-        <f>COUNTIF(Vendas[Região],D5)</f>
+      <c r="B12" s="3">
+        <f>COUNTIF(Vendas[Região],A12)</f>
         <v>12</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="2"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="14" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="24">
+        <f>_xlfn.NUMBERVALUE(SMALL(Vendas[Total],G12))</f>
+        <v>10.981999999999999</v>
+      </c>
+      <c r="I12" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H12,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+      <c r="J12" s="22" t="str">
+        <f>IFERROR((VLOOKUP($H12,Vendas[#All],0,0)),"Not Found")</f>
+        <v>Not Found</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7">
-        <f>COUNTIF(Vendas[Região],D6)</f>
+      <c r="B13" s="3">
+        <f>COUNTIF(Vendas[Região],A13)</f>
         <v>13</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="42">
-      <c r="A8" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4">
-        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!A9,Vendas[Região],Análise!$D$5)</f>
-        <v>326.90999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4">
-        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!A10,Vendas[Região],Análise!$D$5)</f>
-        <v>249.99849999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4">
-        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!A11,Vendas[Região],Análise!$D$5)</f>
-        <v>126.94749999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4">
-        <f>SUMIFS(Vendas[Total],Vendas[Vendedor],Análise!A12,Vendas[Região],Análise!$D$5)</f>
-        <v>100.09699999999999</v>
-      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="6"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="L14" s="18"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="I16" t="e">
+        <f>LOOKUP(H3,Vendas[])</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="13">
+        <f>AVERAGEIF(Vendas[Categoria],A17,Vendas[Total])</f>
+        <v>195.10464999999996</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="20">
+        <f>AVERAGEIFS(Vendas[Total], Vendas[Categoria],A19,Vendas[Trimestre],"1")</f>
+        <v>64.716166666666666</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="13">
+        <f>AVERAGEIF(Vendas[Categoria],A18,Vendas[Total])</f>
+        <v>84.802349999999976</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="13">
+        <f>AVERAGEIF(Vendas[Categoria],A19,Vendas[Total])</f>
+        <v>67.928937499999989</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cellWatches>
+    <cellWatch r="I5"/>
+    <cellWatch r="I3"/>
+  </cellWatches>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
new file:   01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx  	modified:   01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos.xlsx  	modified:   03_Advanced_Internet_Programming/Assignments/001.FilipeMatos/index.html  	new file:   03_Advanced_Internet_Programming/Assignments/Lab01/001.FilipeMatos/SW_Profile.jpg  	new file:   03_Advanced_Internet_Programming/Assignments/Lab01/001.FilipeMatos/index.html  	new file:   03_Advanced_Internet_Programming/Assignments/Lab01/001.FilipeMatos/style.css  	new file:   03_Advanced_Internet_Programming/Assignments/Lab01/01-ReviewLab.pdf
</commit_message>
<xml_diff>
--- a/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos.xlsx
+++ b/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/201600728_estudantes_ips_pt/Documents/02. MEEC/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="8_{89B56B0D-932B-4A63-BBA9-A5E8206EE450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76895314-522F-4C6A-9623-E6419BAB7903}"/>
+  <xr:revisionPtr revIDLastSave="363" documentId="8_{89B56B0D-932B-4A63-BBA9-A5E8206EE450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD92928B-8EB0-4AE4-81A2-F8C3AC46D779}"/>
   <bookViews>
-    <workbookView xWindow="43185" yWindow="-15" windowWidth="14430" windowHeight="15510" activeTab="1" xr2:uid="{C8B6D815-6572-4EFD-9C5A-CC7C1F4CF928}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C8B6D815-6572-4EFD-9C5A-CC7C1F4CF928}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário" sheetId="4" r:id="rId1"/>
@@ -671,10 +671,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1206,30 +1202,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7013D5EB-BEF7-4A56-89FB-305F31E16D24}">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection sqref="A1:P1048576"/>
+    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="24" style="3" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1349,7 +1345,7 @@
       </c>
       <c r="Q2" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="R2" s="26" t="str" cm="1">
         <f t="array" ref="R2">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1413,7 +1409,7 @@
       </c>
       <c r="Q3" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="R3" s="26" t="str" cm="1">
         <f t="array" ref="R3">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1477,7 +1473,7 @@
       </c>
       <c r="Q4" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="R4" s="26" t="str" cm="1">
         <f t="array" ref="R4">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1541,7 +1537,7 @@
       </c>
       <c r="Q5" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="R5" s="26" t="str" cm="1">
         <f t="array" ref="R5">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1605,7 +1601,7 @@
       </c>
       <c r="Q6" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="R6" s="26" t="str" cm="1">
         <f t="array" ref="R6">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1669,7 +1665,7 @@
       </c>
       <c r="Q7" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="R7" s="26" t="str" cm="1">
         <f t="array" ref="R7">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1733,7 +1729,7 @@
       </c>
       <c r="Q8" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="R8" s="26" t="str" cm="1">
         <f t="array" ref="R8">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1797,7 +1793,7 @@
       </c>
       <c r="Q9" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="R9" s="26" t="str" cm="1">
         <f t="array" ref="R9">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1861,7 +1857,7 @@
       </c>
       <c r="Q10" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="R10" s="26" t="str" cm="1">
         <f t="array" ref="R10">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1925,7 +1921,7 @@
       </c>
       <c r="Q11" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="R11" s="26" t="str" cm="1">
         <f t="array" ref="R11">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -1989,7 +1985,7 @@
       </c>
       <c r="Q12" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="R12" s="26" t="str" cm="1">
         <f t="array" ref="R12">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2053,7 +2049,7 @@
       </c>
       <c r="Q13" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="R13" s="26" t="str" cm="1">
         <f t="array" ref="R13">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2117,7 +2113,7 @@
       </c>
       <c r="Q14" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="R14" s="26" t="str" cm="1">
         <f t="array" ref="R14">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2181,7 +2177,7 @@
       </c>
       <c r="Q15" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="R15" s="26" t="str" cm="1">
         <f t="array" ref="R15">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2245,7 +2241,7 @@
       </c>
       <c r="Q16" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="R16" s="26" t="str" cm="1">
         <f t="array" ref="R16">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2309,7 +2305,7 @@
       </c>
       <c r="Q17" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="R17" s="26" t="str" cm="1">
         <f t="array" ref="R17">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2373,7 +2369,7 @@
       </c>
       <c r="Q18" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="R18" s="26" t="str" cm="1">
         <f t="array" ref="R18">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2437,7 +2433,7 @@
       </c>
       <c r="Q19" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="R19" s="26" t="str" cm="1">
         <f t="array" ref="R19">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2501,7 +2497,7 @@
       </c>
       <c r="Q20" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="R20" s="26" t="str" cm="1">
         <f t="array" ref="R20">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2565,7 +2561,7 @@
       </c>
       <c r="Q21" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="R21" s="26" t="str" cm="1">
         <f t="array" ref="R21">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2629,7 +2625,7 @@
       </c>
       <c r="Q22" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="R22" s="26" t="str" cm="1">
         <f t="array" ref="R22">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2693,7 +2689,7 @@
       </c>
       <c r="Q23" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="R23" s="26" t="str" cm="1">
         <f t="array" ref="R23">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2757,7 +2753,7 @@
       </c>
       <c r="Q24" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="R24" s="26" t="str" cm="1">
         <f t="array" ref="R24">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2821,7 +2817,7 @@
       </c>
       <c r="Q25" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="R25" s="26" t="str" cm="1">
         <f t="array" ref="R25">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2885,7 +2881,7 @@
       </c>
       <c r="Q26" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="R26" s="26" t="str" cm="1">
         <f t="array" ref="R26">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -2949,7 +2945,7 @@
       </c>
       <c r="Q27" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="R27" s="26" t="str" cm="1">
         <f t="array" ref="R27">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3013,7 +3009,7 @@
       </c>
       <c r="Q28" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="R28" s="26" t="str" cm="1">
         <f t="array" ref="R28">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3077,7 +3073,7 @@
       </c>
       <c r="Q29" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="R29" s="26" t="str" cm="1">
         <f t="array" ref="R29">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3141,7 +3137,7 @@
       </c>
       <c r="Q30" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="R30" s="26" t="str" cm="1">
         <f t="array" ref="R30">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3205,7 +3201,7 @@
       </c>
       <c r="Q31" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="R31" s="26" t="str" cm="1">
         <f t="array" ref="R31">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3269,7 +3265,7 @@
       </c>
       <c r="Q32" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="R32" s="26" t="str" cm="1">
         <f t="array" ref="R32">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3333,7 +3329,7 @@
       </c>
       <c r="Q33" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="R33" s="26" t="str" cm="1">
         <f t="array" ref="R33">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3397,7 +3393,7 @@
       </c>
       <c r="Q34" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="R34" s="26" t="str" cm="1">
         <f t="array" ref="R34">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3461,7 +3457,7 @@
       </c>
       <c r="Q35" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="R35" s="26" t="str" cm="1">
         <f t="array" ref="R35">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3525,7 +3521,7 @@
       </c>
       <c r="Q36" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="R36" s="26" t="str" cm="1">
         <f t="array" ref="R36">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3589,7 +3585,7 @@
       </c>
       <c r="Q37" s="6">
         <f ca="1">TODAY()-Vendas[[#This Row],[Data]]</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R37" s="26" t="str" cm="1">
         <f t="array" ref="R37">_xlfn.IFS(Vendas[[#This Row],[Total]]&gt;=250, "Alto", AND(Vendas[[#This Row],[Total]]&gt;=100, Vendas[[#This Row],[Total]]&lt;=249.99), "Médio", Vendas[[#This Row],[Total]]&lt;100,"Baixo")</f>
@@ -3613,8 +3609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E298A1-41BF-485F-AE78-098E1D130449}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>